<commit_message>
am pus o noue linie in excel
</commit_message>
<xml_diff>
--- a/git_commands.xlsx
+++ b/git_commands.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\python_exercise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S1DLD78\Desktop\Stuff\13_Scripts_Python\python_exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DBBE90-45C6-43EF-891E-2685E9110400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C1BFC1-00CE-462C-B600-2519E070AFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-105" windowWidth="29040" windowHeight="15990" xr2:uid="{AB59D656-62A4-4798-9317-6852DA1E6397}"/>
+    <workbookView xWindow="32640" yWindow="2760" windowWidth="15945" windowHeight="9750" xr2:uid="{AB59D656-62A4-4798-9317-6852DA1E6397}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Comenzi Git</t>
   </si>
@@ -50,9 +50,6 @@
     <t>aduce pe local un repo nou</t>
   </si>
   <si>
-    <t>git checkout -b nume_branch</t>
-  </si>
-  <si>
     <t xml:space="preserve">creeaza un branch nou </t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>creeaza un branch nou si te muta pe acel branch</t>
   </si>
   <si>
-    <t>git branch nume_branch</t>
-  </si>
-  <si>
     <t xml:space="preserve">duce schimbarile pe online </t>
   </si>
   <si>
@@ -102,6 +96,18 @@
   </si>
   <si>
     <t>observa schimbarile de pe server - doar de pe branchul curent</t>
+  </si>
+  <si>
+    <t>git reset --hard origin/&lt;nume_branch&gt;</t>
+  </si>
+  <si>
+    <t>reseteaza branch-ul local, ca sa fie ca pe online</t>
+  </si>
+  <si>
+    <t>git branch &lt;nume_branch&gt;</t>
+  </si>
+  <si>
+    <t>git checkout -b &lt;nume_branch&gt;</t>
   </si>
 </sst>
 </file>
@@ -149,10 +155,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,19 +494,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB7C27B-10F7-486D-9332-08674599D5A1}">
-  <dimension ref="B1:C12"/>
+  <dimension ref="B1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" customWidth="1"/>
     <col min="3" max="3" width="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -507,7 +514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -515,76 +522,84 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="2" t="s">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update aexcel and aded main to py
</commit_message>
<xml_diff>
--- a/git_commands.xlsx
+++ b/git_commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S1DLD78\Desktop\Stuff\13_Scripts_Python\python_exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C1BFC1-00CE-462C-B600-2519E070AFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDABBE9B-34B6-4FFC-89EC-9BCF8052B763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32640" yWindow="2760" windowWidth="15945" windowHeight="9750" xr2:uid="{AB59D656-62A4-4798-9317-6852DA1E6397}"/>
+    <workbookView xWindow="32295" yWindow="2415" windowWidth="15945" windowHeight="9750" xr2:uid="{AB59D656-62A4-4798-9317-6852DA1E6397}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Comenzi Git</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>git checkout -b &lt;nume_branch&gt;</t>
+  </si>
+  <si>
+    <t>git branch</t>
+  </si>
+  <si>
+    <t>list of all branches</t>
   </si>
 </sst>
 </file>
@@ -494,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB7C27B-10F7-486D-9332-08674599D5A1}">
-  <dimension ref="B1:C13"/>
+  <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,11 +601,19 @@
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>